<commit_message>
Primera fila fixada del excel
</commit_message>
<xml_diff>
--- a/service-flask/voluntariat_app/xlsx/template.xlsx
+++ b/service-flask/voluntariat_app/xlsx/template.xlsx
@@ -196,10 +196,12 @@
   <dimension ref="AMH1:AMJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AMH1" s="2"/>

</xml_diff>